<commit_message>
PROS-7671 - update KPI POS
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - FT - CAP.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - FT - CAP.xlsx
@@ -12,16 +12,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1067,10 +1058,10 @@
     <t xml:space="preserve">Прикассовый дисплеи Entry Pack фейсы</t>
   </si>
   <si>
-    <t xml:space="preserve">Coca-Cola - 0.25L Slim, Coca-Cola Zero - 0.25L Slim, Coca-Cola Zero Cherry - 0.25L Slim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5449000008046, 5449000020987, 5449000239655</t>
+    <t xml:space="preserve">Coca-Cola - 0.25L Slim, Coca-Cola Zero - 0.25L Slim, Coca-Cola Zero Cherry - 0.25L Slim, Sprite - 0.25L Slim, Fanta Orange - 0.25L Slim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000008046, 5449000020987, 5449000239655, 5449000000729, 5449000000712</t>
   </si>
   <si>
     <t xml:space="preserve">Entry_Pack</t>
@@ -1715,11 +1706,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1827,54 +1818,56 @@
   </sheetPr>
   <dimension ref="A1:BD115"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="M38" activeCellId="0" sqref="M38:N38"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="22.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="48.2024291497976"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="69.3076923076923"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="44.0242914979757"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="45.5263157894737"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="43.7044534412956"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="49.165991902834"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="96.5141700404858"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="86.336032388664"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3036437246964"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8259109311741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.9514170040486"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4898785425101"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5627530364372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="47.1093117408907"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="67.2995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="43.0404858299595"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.7449392712551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.45344129554656"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.6963562753036"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.2024291497976"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="114.283400809717"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="71.3684210526316"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.2955465587045"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="14.0323886639676"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="7.24696356275304"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="14.7125506072875"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.9392712550607"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="22.3441295546559"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="47.9595141700405"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="23.8744939271255"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="25.9068825910931"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="26.417004048583"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="26.7570850202429"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="13.6963562753036"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="12.8461538461538"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="13.3522267206478"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="51.8582995951417"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="83.9230769230769"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="7.92712550607287"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="9.11336032388664"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="11.1457489878543"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="9.62753036437247"/>
+    <col collapsed="false" hidden="false" max="1025" min="39" style="1" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1991,7 +1984,7 @@
       </c>
       <c r="BD1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="n">
         <v>174</v>
       </c>
@@ -2052,7 +2045,7 @@
       <c r="AL2" s="6"/>
       <c r="BD2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="n">
         <v>175</v>
       </c>
@@ -2113,7 +2106,7 @@
       <c r="AL3" s="10"/>
       <c r="BD3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
         <v>176</v>
       </c>
@@ -2176,7 +2169,7 @@
       </c>
       <c r="BD4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="n">
         <v>177</v>
       </c>
@@ -2239,7 +2232,7 @@
       </c>
       <c r="BD5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="n">
         <v>178</v>
       </c>
@@ -2300,7 +2293,7 @@
       <c r="AL6" s="10"/>
       <c r="BD6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="n">
         <v>179</v>
       </c>
@@ -2363,7 +2356,7 @@
       </c>
       <c r="BD7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
         <v>180</v>
       </c>
@@ -2426,7 +2419,7 @@
       </c>
       <c r="BD8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
         <v>182</v>
       </c>
@@ -2489,7 +2482,7 @@
       </c>
       <c r="BD9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
         <v>183</v>
       </c>
@@ -2552,7 +2545,7 @@
       </c>
       <c r="BD10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="n">
         <v>184</v>
       </c>
@@ -2615,7 +2608,7 @@
       </c>
       <c r="BD11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
         <v>185</v>
       </c>
@@ -2678,7 +2671,7 @@
       </c>
       <c r="BD12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
         <v>186</v>
       </c>
@@ -2741,7 +2734,7 @@
       </c>
       <c r="BD13" s="0"/>
     </row>
-    <row r="14" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
         <v>188</v>
       </c>
@@ -2802,7 +2795,7 @@
       <c r="AL14" s="6"/>
       <c r="BD14" s="0"/>
     </row>
-    <row r="15" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
         <v>1</v>
       </c>
@@ -2869,7 +2862,7 @@
       </c>
       <c r="BD15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
         <v>2</v>
       </c>
@@ -2950,7 +2943,7 @@
       </c>
       <c r="BD16" s="0"/>
     </row>
-    <row r="17" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
         <v>3</v>
       </c>
@@ -3031,7 +3024,7 @@
       </c>
       <c r="BD17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="n">
         <v>4</v>
       </c>
@@ -3112,7 +3105,7 @@
       </c>
       <c r="BD18" s="0"/>
     </row>
-    <row r="19" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="n">
         <v>5</v>
       </c>
@@ -3193,7 +3186,7 @@
       </c>
       <c r="BD19" s="0"/>
     </row>
-    <row r="20" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="n">
         <v>6</v>
       </c>
@@ -3274,7 +3267,7 @@
       </c>
       <c r="BD20" s="0"/>
     </row>
-    <row r="21" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="n">
         <v>7</v>
       </c>
@@ -3355,7 +3348,7 @@
       </c>
       <c r="BD21" s="0"/>
     </row>
-    <row r="22" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="n">
         <v>8</v>
       </c>
@@ -3436,7 +3429,7 @@
       </c>
       <c r="BD22" s="0"/>
     </row>
-    <row r="23" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="n">
         <v>9</v>
       </c>
@@ -3517,7 +3510,7 @@
       </c>
       <c r="BD23" s="0"/>
     </row>
-    <row r="24" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="n">
         <v>10</v>
       </c>
@@ -3598,7 +3591,7 @@
       </c>
       <c r="BD24" s="0"/>
     </row>
-    <row r="25" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="n">
         <v>11</v>
       </c>
@@ -3679,7 +3672,7 @@
       </c>
       <c r="BD25" s="0"/>
     </row>
-    <row r="26" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="n">
         <v>12</v>
       </c>
@@ -3760,7 +3753,7 @@
       </c>
       <c r="BD26" s="0"/>
     </row>
-    <row r="27" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="n">
         <v>13</v>
       </c>
@@ -3841,7 +3834,7 @@
       </c>
       <c r="BD27" s="0"/>
     </row>
-    <row r="28" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="n">
         <v>14</v>
       </c>
@@ -3922,7 +3915,7 @@
       </c>
       <c r="BD28" s="0"/>
     </row>
-    <row r="29" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="n">
         <v>15</v>
       </c>
@@ -4003,7 +3996,7 @@
       </c>
       <c r="BD29" s="0"/>
     </row>
-    <row r="30" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="n">
         <v>16</v>
       </c>
@@ -4084,7 +4077,7 @@
       </c>
       <c r="BD30" s="0"/>
     </row>
-    <row r="31" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="n">
         <v>17</v>
       </c>
@@ -4165,7 +4158,7 @@
       </c>
       <c r="BD31" s="0"/>
     </row>
-    <row r="32" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="n">
         <v>18</v>
       </c>
@@ -4246,7 +4239,7 @@
       </c>
       <c r="BD32" s="0"/>
     </row>
-    <row r="33" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="n">
         <v>19</v>
       </c>
@@ -4327,7 +4320,7 @@
       </c>
       <c r="BD33" s="0"/>
     </row>
-    <row r="34" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="n">
         <v>20</v>
       </c>
@@ -4408,7 +4401,7 @@
       </c>
       <c r="BD34" s="0"/>
     </row>
-    <row r="35" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="n">
         <v>21</v>
       </c>
@@ -4489,7 +4482,7 @@
       </c>
       <c r="BD35" s="0"/>
     </row>
-    <row r="36" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="n">
         <v>22</v>
       </c>
@@ -4570,7 +4563,7 @@
       </c>
       <c r="BD36" s="0"/>
     </row>
-    <row r="37" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="n">
         <v>23</v>
       </c>
@@ -4651,7 +4644,7 @@
       </c>
       <c r="BD37" s="0"/>
     </row>
-    <row r="38" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="n">
         <v>24</v>
       </c>
@@ -4732,7 +4725,7 @@
       </c>
       <c r="BD38" s="0"/>
     </row>
-    <row r="39" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="n">
         <v>25</v>
       </c>
@@ -4799,7 +4792,7 @@
       </c>
       <c r="BD39" s="0"/>
     </row>
-    <row r="40" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="n">
         <v>26</v>
       </c>
@@ -4880,7 +4873,7 @@
       </c>
       <c r="BD40" s="0"/>
     </row>
-    <row r="41" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="n">
         <v>27</v>
       </c>
@@ -4961,7 +4954,7 @@
       </c>
       <c r="BD41" s="0"/>
     </row>
-    <row r="42" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="n">
         <v>28</v>
       </c>
@@ -5042,7 +5035,7 @@
       </c>
       <c r="BD42" s="0"/>
     </row>
-    <row r="43" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="n">
         <v>29</v>
       </c>
@@ -5123,7 +5116,7 @@
       </c>
       <c r="BD43" s="0"/>
     </row>
-    <row r="44" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="n">
         <v>30</v>
       </c>
@@ -5204,7 +5197,7 @@
       </c>
       <c r="BD44" s="0"/>
     </row>
-    <row r="45" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="n">
         <v>31</v>
       </c>
@@ -5285,7 +5278,7 @@
       </c>
       <c r="BD45" s="0"/>
     </row>
-    <row r="46" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="n">
         <v>32</v>
       </c>
@@ -5352,7 +5345,7 @@
       </c>
       <c r="BD46" s="0"/>
     </row>
-    <row r="47" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="n">
         <v>33</v>
       </c>
@@ -5433,7 +5426,7 @@
       </c>
       <c r="BD47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="n">
         <v>34</v>
       </c>
@@ -5514,7 +5507,7 @@
       </c>
       <c r="BD48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="n">
         <v>35</v>
       </c>
@@ -5595,7 +5588,7 @@
       </c>
       <c r="BD49" s="0"/>
     </row>
-    <row r="50" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="n">
         <v>36</v>
       </c>
@@ -5676,7 +5669,7 @@
       </c>
       <c r="BD50" s="0"/>
     </row>
-    <row r="51" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="n">
         <v>37</v>
       </c>
@@ -5757,7 +5750,7 @@
       </c>
       <c r="BD51" s="0"/>
     </row>
-    <row r="52" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="n">
         <v>38</v>
       </c>
@@ -5824,7 +5817,7 @@
       </c>
       <c r="BD52" s="0"/>
     </row>
-    <row r="53" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="n">
         <v>39</v>
       </c>
@@ -5905,7 +5898,7 @@
       </c>
       <c r="BD53" s="0"/>
     </row>
-    <row r="54" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="n">
         <v>40</v>
       </c>
@@ -5986,7 +5979,7 @@
       </c>
       <c r="BD54" s="0"/>
     </row>
-    <row r="55" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="n">
         <v>41</v>
       </c>
@@ -6067,7 +6060,7 @@
       </c>
       <c r="BD55" s="0"/>
     </row>
-    <row r="56" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="n">
         <v>42</v>
       </c>
@@ -6148,7 +6141,7 @@
       </c>
       <c r="BD56" s="0"/>
     </row>
-    <row r="57" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="n">
         <v>43</v>
       </c>
@@ -6229,7 +6222,7 @@
       </c>
       <c r="BD57" s="0"/>
     </row>
-    <row r="58" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="n">
         <v>44</v>
       </c>
@@ -6310,7 +6303,7 @@
       </c>
       <c r="BD58" s="0"/>
     </row>
-    <row r="59" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="n">
         <v>45</v>
       </c>
@@ -6377,7 +6370,7 @@
       </c>
       <c r="BD59" s="0"/>
     </row>
-    <row r="60" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="n">
         <v>46</v>
       </c>
@@ -6458,7 +6451,7 @@
       </c>
       <c r="BD60" s="0"/>
     </row>
-    <row r="61" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="n">
         <v>47</v>
       </c>
@@ -6539,7 +6532,7 @@
       </c>
       <c r="BD61" s="0"/>
     </row>
-    <row r="62" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="n">
         <v>48</v>
       </c>
@@ -6620,7 +6613,7 @@
       </c>
       <c r="BD62" s="0"/>
     </row>
-    <row r="63" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="n">
         <v>49</v>
       </c>
@@ -6701,7 +6694,7 @@
       </c>
       <c r="BD63" s="0"/>
     </row>
-    <row r="64" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="n">
         <v>50</v>
       </c>
@@ -6782,7 +6775,7 @@
       </c>
       <c r="BD64" s="0"/>
     </row>
-    <row r="65" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="n">
         <v>51</v>
       </c>
@@ -6863,7 +6856,7 @@
       </c>
       <c r="BD65" s="0"/>
     </row>
-    <row r="66" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="n">
         <v>52</v>
       </c>
@@ -6944,7 +6937,7 @@
       </c>
       <c r="BD66" s="0"/>
     </row>
-    <row r="67" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="n">
         <v>53</v>
       </c>
@@ -7025,7 +7018,7 @@
       </c>
       <c r="BD67" s="0"/>
     </row>
-    <row r="68" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="n">
         <v>54</v>
       </c>
@@ -7106,7 +7099,7 @@
       </c>
       <c r="BD68" s="0"/>
     </row>
-    <row r="69" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="n">
         <v>55</v>
       </c>
@@ -7187,7 +7180,7 @@
       </c>
       <c r="BD69" s="0"/>
     </row>
-    <row r="70" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="n">
         <v>56</v>
       </c>
@@ -7268,7 +7261,7 @@
       </c>
       <c r="BD70" s="0"/>
     </row>
-    <row r="71" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="n">
         <v>57</v>
       </c>
@@ -7349,7 +7342,7 @@
       </c>
       <c r="BD71" s="0"/>
     </row>
-    <row r="72" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="n">
         <v>58</v>
       </c>
@@ -7426,7 +7419,7 @@
       </c>
       <c r="BD72" s="0"/>
     </row>
-    <row r="73" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="n">
         <v>59</v>
       </c>
@@ -7501,7 +7494,7 @@
       </c>
       <c r="BD73" s="0"/>
     </row>
-    <row r="74" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="n">
         <v>60</v>
       </c>
@@ -7576,7 +7569,7 @@
       </c>
       <c r="BD74" s="0"/>
     </row>
-    <row r="75" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="n">
         <v>61</v>
       </c>
@@ -7651,7 +7644,7 @@
       </c>
       <c r="BD75" s="0"/>
     </row>
-    <row r="76" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="n">
         <v>62</v>
       </c>
@@ -7726,7 +7719,7 @@
       </c>
       <c r="BD76" s="0"/>
     </row>
-    <row r="77" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="n">
         <v>63</v>
       </c>
@@ -7801,7 +7794,7 @@
       </c>
       <c r="BD77" s="0"/>
     </row>
-    <row r="78" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="n">
         <v>64</v>
       </c>
@@ -7878,7 +7871,7 @@
       </c>
       <c r="BD78" s="0"/>
     </row>
-    <row r="79" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="n">
         <v>65</v>
       </c>
@@ -7951,7 +7944,7 @@
       </c>
       <c r="BD79" s="0"/>
     </row>
-    <row r="80" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="n">
         <v>66</v>
       </c>
@@ -8030,7 +8023,7 @@
       </c>
       <c r="BD80" s="0"/>
     </row>
-    <row r="81" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="n">
         <v>69</v>
       </c>
@@ -8105,7 +8098,7 @@
       </c>
       <c r="BD81" s="0"/>
     </row>
-    <row r="82" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="n">
         <v>70</v>
       </c>
@@ -8182,7 +8175,7 @@
       </c>
       <c r="BD82" s="0"/>
     </row>
-    <row r="83" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="6" t="n">
         <v>71</v>
       </c>
@@ -8255,7 +8248,7 @@
       </c>
       <c r="BD83" s="0"/>
     </row>
-    <row r="84" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="n">
         <v>72</v>
       </c>
@@ -8332,7 +8325,7 @@
       </c>
       <c r="BD84" s="0"/>
     </row>
-    <row r="85" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="n">
         <v>73</v>
       </c>
@@ -8409,7 +8402,7 @@
       </c>
       <c r="BD85" s="0"/>
     </row>
-    <row r="86" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="n">
         <v>74</v>
       </c>
@@ -8484,7 +8477,7 @@
       </c>
       <c r="BD86" s="0"/>
     </row>
-    <row r="87" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="n">
         <v>75</v>
       </c>
@@ -8512,7 +8505,7 @@
       <c r="K87" s="6"/>
       <c r="L87" s="6"/>
       <c r="M87" s="6"/>
-      <c r="N87" s="23" t="s">
+      <c r="N87" s="10" t="s">
         <v>308</v>
       </c>
       <c r="O87" s="10"/>
@@ -8559,7 +8552,7 @@
       </c>
       <c r="BD87" s="0"/>
     </row>
-    <row r="88" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="n">
         <v>76</v>
       </c>
@@ -8587,7 +8580,7 @@
       <c r="K88" s="6"/>
       <c r="L88" s="6"/>
       <c r="M88" s="6"/>
-      <c r="N88" s="24"/>
+      <c r="N88" s="6"/>
       <c r="O88" s="10"/>
       <c r="P88" s="10"/>
       <c r="Q88" s="6"/>
@@ -8628,7 +8621,7 @@
       </c>
       <c r="BD88" s="0"/>
     </row>
-    <row r="89" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="6" t="n">
         <v>77</v>
       </c>
@@ -8655,10 +8648,10 @@
       </c>
       <c r="K89" s="6"/>
       <c r="L89" s="6"/>
-      <c r="M89" s="6" t="s">
+      <c r="M89" s="23" t="s">
         <v>320</v>
       </c>
-      <c r="N89" s="23" t="s">
+      <c r="N89" s="24" t="s">
         <v>321</v>
       </c>
       <c r="O89" s="10"/>
@@ -8701,7 +8694,7 @@
       </c>
       <c r="BD89" s="0"/>
     </row>
-    <row r="90" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="6" t="n">
         <v>78</v>
       </c>
@@ -8729,7 +8722,7 @@
       <c r="K90" s="6"/>
       <c r="L90" s="6"/>
       <c r="M90" s="6"/>
-      <c r="N90" s="24"/>
+      <c r="N90" s="6"/>
       <c r="O90" s="10"/>
       <c r="P90" s="10"/>
       <c r="Q90" s="6"/>
@@ -8770,7 +8763,7 @@
       </c>
       <c r="BD90" s="0"/>
     </row>
-    <row r="91" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="6" t="n">
         <v>79</v>
       </c>
@@ -8843,7 +8836,7 @@
       </c>
       <c r="BD91" s="0"/>
     </row>
-    <row r="92" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="6" t="n">
         <v>80</v>
       </c>
@@ -8926,7 +8919,7 @@
       </c>
       <c r="BD92" s="0"/>
     </row>
-    <row r="93" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="6" t="n">
         <v>81</v>
       </c>
@@ -9009,7 +9002,7 @@
       </c>
       <c r="BD93" s="0"/>
     </row>
-    <row r="94" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="6" t="n">
         <v>82</v>
       </c>
@@ -9084,7 +9077,7 @@
       </c>
       <c r="BD94" s="0"/>
     </row>
-    <row r="95" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="6" t="n">
         <v>83</v>
       </c>
@@ -9165,7 +9158,7 @@
       </c>
       <c r="BD95" s="0"/>
     </row>
-    <row r="96" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="6" t="n">
         <v>84</v>
       </c>
@@ -9250,7 +9243,7 @@
       </c>
       <c r="BD96" s="0"/>
     </row>
-    <row r="97" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="6" t="n">
         <v>85</v>
       </c>
@@ -9331,7 +9324,7 @@
       </c>
       <c r="BD97" s="0"/>
     </row>
-    <row r="98" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="6" t="n">
         <v>87</v>
       </c>
@@ -9414,7 +9407,7 @@
       </c>
       <c r="BD98" s="0"/>
     </row>
-    <row r="99" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="6" t="n">
         <v>88</v>
       </c>
@@ -9489,7 +9482,7 @@
       </c>
       <c r="BD99" s="0"/>
     </row>
-    <row r="100" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="6" t="n">
         <v>89</v>
       </c>
@@ -9506,7 +9499,7 @@
       <c r="F100" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="G100" s="24" t="s">
+      <c r="G100" s="23" t="s">
         <v>373</v>
       </c>
       <c r="H100" s="6" t="s">
@@ -9518,14 +9511,14 @@
       </c>
       <c r="K100" s="6"/>
       <c r="L100" s="0"/>
-      <c r="M100" s="24" t="s">
+      <c r="M100" s="23" t="s">
         <v>374</v>
       </c>
-      <c r="N100" s="23" t="s">
+      <c r="N100" s="24" t="s">
         <v>375</v>
       </c>
-      <c r="O100" s="23"/>
-      <c r="P100" s="23" t="s">
+      <c r="O100" s="24"/>
+      <c r="P100" s="24" t="s">
         <v>375</v>
       </c>
       <c r="Q100" s="6" t="s">
@@ -9574,7 +9567,7 @@
       </c>
       <c r="BD100" s="0"/>
     </row>
-    <row r="101" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="6" t="n">
         <v>90</v>
       </c>
@@ -9591,7 +9584,7 @@
       <c r="F101" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="G101" s="24" t="s">
+      <c r="G101" s="23" t="s">
         <v>379</v>
       </c>
       <c r="H101" s="6" t="s">
@@ -9603,14 +9596,14 @@
       </c>
       <c r="K101" s="6"/>
       <c r="L101" s="6"/>
-      <c r="M101" s="24" t="s">
+      <c r="M101" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="N101" s="23" t="s">
+      <c r="N101" s="24" t="s">
         <v>367</v>
       </c>
-      <c r="O101" s="23"/>
-      <c r="P101" s="23" t="s">
+      <c r="O101" s="24"/>
+      <c r="P101" s="24" t="s">
         <v>367</v>
       </c>
       <c r="Q101" s="6" t="s">
@@ -9659,7 +9652,7 @@
       </c>
       <c r="BD101" s="0"/>
     </row>
-    <row r="102" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="6" t="n">
         <v>91</v>
       </c>
@@ -9740,7 +9733,7 @@
       </c>
       <c r="BD102" s="0"/>
     </row>
-    <row r="103" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="6" t="n">
         <v>92</v>
       </c>
@@ -9817,7 +9810,7 @@
       </c>
       <c r="BD103" s="0"/>
     </row>
-    <row r="104" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="6" t="n">
         <v>93</v>
       </c>
@@ -9888,7 +9881,7 @@
       <c r="AL104" s="6"/>
       <c r="BD104" s="0"/>
     </row>
-    <row r="105" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="6" t="n">
         <v>94</v>
       </c>
@@ -9920,7 +9913,7 @@
       <c r="K105" s="6"/>
       <c r="L105" s="6"/>
       <c r="M105" s="6"/>
-      <c r="N105" s="24" t="s">
+      <c r="N105" s="23" t="s">
         <v>311</v>
       </c>
       <c r="O105" s="6"/>
@@ -9955,7 +9948,7 @@
       <c r="AL105" s="6"/>
       <c r="BD105" s="0"/>
     </row>
-    <row r="106" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="6" t="n">
         <v>95</v>
       </c>
@@ -9987,7 +9980,7 @@
       <c r="K106" s="6"/>
       <c r="L106" s="6"/>
       <c r="M106" s="6"/>
-      <c r="N106" s="24" t="s">
+      <c r="N106" s="23" t="s">
         <v>316</v>
       </c>
       <c r="O106" s="6"/>
@@ -10022,7 +10015,7 @@
       <c r="AL106" s="6"/>
       <c r="BD106" s="0"/>
     </row>
-    <row r="107" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="6" t="n">
         <v>96</v>
       </c>
@@ -10054,7 +10047,7 @@
       <c r="K107" s="6"/>
       <c r="L107" s="6"/>
       <c r="M107" s="6"/>
-      <c r="N107" s="24" t="s">
+      <c r="N107" s="23" t="s">
         <v>322</v>
       </c>
       <c r="O107" s="6"/>
@@ -10089,7 +10082,7 @@
       <c r="AL107" s="6"/>
       <c r="BD107" s="0"/>
     </row>
-    <row r="108" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="6" t="n">
         <v>97</v>
       </c>
@@ -10121,7 +10114,7 @@
       <c r="K108" s="6"/>
       <c r="L108" s="6"/>
       <c r="M108" s="6"/>
-      <c r="N108" s="24" t="s">
+      <c r="N108" s="23" t="s">
         <v>325</v>
       </c>
       <c r="O108" s="6"/>
@@ -10156,7 +10149,7 @@
       <c r="AL108" s="6"/>
       <c r="BD108" s="0"/>
     </row>
-    <row r="109" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="6" t="n">
         <v>98</v>
       </c>
@@ -10225,7 +10218,7 @@
       <c r="AL109" s="6"/>
       <c r="BD109" s="28"/>
     </row>
-    <row r="110" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="6" t="n">
         <v>99</v>
       </c>
@@ -10291,7 +10284,7 @@
       <c r="AK110" s="6"/>
       <c r="AL110" s="6"/>
     </row>
-    <row r="111" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="6" t="n">
         <v>100</v>
       </c>
@@ -10357,7 +10350,7 @@
       <c r="AK111" s="6"/>
       <c r="AL111" s="6"/>
     </row>
-    <row r="112" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="6" t="n">
         <v>101</v>
       </c>
@@ -10423,7 +10416,7 @@
       <c r="AK112" s="6"/>
       <c r="AL112" s="6"/>
     </row>
-    <row r="113" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="6" t="n">
         <v>102</v>
       </c>
@@ -10491,7 +10484,7 @@
       </c>
       <c r="AL113" s="6"/>
     </row>
-    <row r="114" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="6" t="n">
         <v>103</v>
       </c>
@@ -10559,7 +10552,7 @@
       </c>
       <c r="AL114" s="6"/>
     </row>
-    <row r="115" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="6" t="n">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
PROS-7196 - CCRU - Ext Planned Visits - Development
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - FT - CAP.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - FT - CAP.xlsx
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$115</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="430">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -1446,6 +1447,15 @@
   <si>
     <t xml:space="preserve">OTG
 No_O_A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer</t>
   </si>
 </sst>
 </file>
@@ -1851,54 +1861,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BD115"/>
+  <dimension ref="A1:BD116"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F44" activeCellId="0" sqref="F44"/>
+      <selection pane="bottomLeft" activeCell="A116" activeCellId="0" sqref="116:116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="48.3117408906883"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="68.9838056680162"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="44.1336032388664"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="48.7408906882591"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="69.6275303643725"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="44.4534412955466"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="2" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="117.51012145749"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="73.2712550607288"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="118.578947368421"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="73.8056680161943"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="1" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="1" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="49.2753036437247"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="27.1012145748988"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="49.5951417004049"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="27.3157894736842"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="32" min="32" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="53.2388663967611"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="86.0161943319838"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="86.7651821862348"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="1" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="36" min="36" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="1023" min="39" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.10526315789474"/>
   </cols>
@@ -10650,6 +10660,66 @@
       <c r="AK115" s="8"/>
       <c r="AL115" s="8"/>
     </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="8" t="n">
+        <v>521</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="E116" s="29"/>
+      <c r="F116" s="29" t="s">
+        <v>427</v>
+      </c>
+      <c r="G116" s="29" t="s">
+        <v>428</v>
+      </c>
+      <c r="H116" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="I116" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="J116" s="10"/>
+      <c r="K116" s="10"/>
+      <c r="L116" s="10"/>
+      <c r="M116" s="8"/>
+      <c r="N116" s="37"/>
+      <c r="O116" s="8"/>
+      <c r="P116" s="8"/>
+      <c r="Q116" s="8"/>
+      <c r="R116" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="S116" s="8"/>
+      <c r="T116" s="8"/>
+      <c r="U116" s="8"/>
+      <c r="V116" s="8"/>
+      <c r="W116" s="8"/>
+      <c r="X116" s="8"/>
+      <c r="Y116" s="8"/>
+      <c r="Z116" s="8"/>
+      <c r="AA116" s="8"/>
+      <c r="AB116" s="8"/>
+      <c r="AC116" s="8"/>
+      <c r="AD116" s="11"/>
+      <c r="AE116" s="8"/>
+      <c r="AF116" s="8"/>
+      <c r="AG116" s="8"/>
+      <c r="AH116" s="8"/>
+      <c r="AI116" s="8"/>
+      <c r="AJ116" s="8" t="n">
+        <v>521</v>
+      </c>
+      <c r="AK116" s="8"/>
+      <c r="AL116" s="8"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AL115"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
PROS-12983 - CCRU - Wrong KPI calculation
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - FT - CAP.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - FT - CAP.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuri\Downloads\0212\PoS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My folder\RED\POS 2019\POS_2019-12-16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDE0294-03AF-46B4-BA49-B73C95130378}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5D8085-906C-45AD-A2FD-D9A631CDD3AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="742" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="742" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traditional Trade" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_FilterDatabase_0" localSheetId="0">'Traditional Trade'!$A$1:$AN$103</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="0">'Traditional Trade'!$A$1:$AN$103</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -917,9 +917,6 @@
     <t>0.2, 0.11</t>
   </si>
   <si>
-    <t>Dobry 0.2, SS_Dobry 0.2</t>
-  </si>
-  <si>
     <t>Cashier Displays Dobry 0.2 Zone</t>
   </si>
   <si>
@@ -932,9 +929,6 @@
     <t>NUM_SCENES</t>
   </si>
   <si>
-    <t>Dobry 0.2_Zone, SS_Dobry 0.2_Zone</t>
-  </si>
-  <si>
     <t>Calculate only if passed KPI Cashier Displays Dobry 0.2</t>
   </si>
   <si>
@@ -950,16 +944,10 @@
     <t>5449000008046, 5449000020987, 5449000239655, 5449000000729, 5449000000712</t>
   </si>
   <si>
-    <t>Entry_Pack, SS_Dobry 0.2_Zone</t>
-  </si>
-  <si>
     <t>Cashier Displays Entry Pack Zone</t>
   </si>
   <si>
     <t>Прикассовый дисплеи Entry Pack Зона</t>
-  </si>
-  <si>
-    <t>Entry_PacK_ Zone, SS_Dobry 0.2_Zone</t>
   </si>
   <si>
     <t>Calculate only if passed KPI Cashier Displays Entry Pack</t>
@@ -1106,9 +1094,6 @@
     <t>Coca-Cola</t>
   </si>
   <si>
-    <t>SSD 1 door, SSD 1.5 door, Mixed 1 door, Mixed  1.5 door, SS_SSD 1 door, SS_SSD 1.5 door, SS_Mixed 1 door, SS_Mixed  1.5 door</t>
-  </si>
-  <si>
     <t>Cooler: Merch Priorty STD fuze and coca- cola shelf 2-3</t>
   </si>
   <si>
@@ -1129,9 +1114,6 @@
   </si>
   <si>
     <t>Fuzetea</t>
-  </si>
-  <si>
-    <t>SSD 1 door, NCB 1 door, Mixed 1 door, SSD 1.5 door, NSB  1.5 door, Mixed  1.5 door, SSDFL 1 door, SSDFL 1.5 door, SS_SSD 1 door, SS_NCB 1 door, SS_Mixed 1 door, SS_SSD 1.5 door, SS_NSB  1.5 door, SS_Mixed  1.5 door, SS_SSDFL 1 door, SS_SSDFL 1.5 door</t>
   </si>
   <si>
     <t>2,3</t>
@@ -1240,9 +1222,6 @@
     <t>SCENE LEVEL</t>
   </si>
   <si>
-    <t>SSD 1 door, NSB 1 door, Mixed 1 door, FC 1 door, SSD 1.5 door, NSB  1.5 door, Mixed  1.5 door, FC door 1.5 door</t>
-  </si>
-  <si>
     <t>Attribute 1</t>
   </si>
   <si>
@@ -1256,9 +1235,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>Freezer BIG SSD, SSD Cooler-Side Rack Big, SSD Cooler-Side Rack Small, SSD Mini pallet, SSD Neck-hanging Rack, Freezer Small SSD, Other SSD Display BIG, Other SSD Display Small, Juice Cooler-Side Rack, Juice Freezer, Juice Mini Pallet, Other Juice Display BIG, Pulpy Cooler-Side Rack, Pulpy Other, Other Juice Display Small, Bonaqua Display, Fuzetea Display, Energy Display, Promo SSD, Promo Juice, Promo Water, Promo Energy, Promo Fuzetea</t>
   </si>
   <si>
     <t>Scene Sub Type 1</t>
@@ -1311,12 +1287,6 @@
     <t>Integer</t>
   </si>
   <si>
-    <t>Panoramic Photo, SS_Panoramic Photo</t>
-  </si>
-  <si>
-    <t>Panoramic photo of Cooler, SS_Panoramic photo of Cooler - Traditional Trade</t>
-  </si>
-  <si>
     <t>Category KPI Type</t>
   </si>
   <si>
@@ -1327,6 +1297,36 @@
   </si>
   <si>
     <t>Schweppes Bitter Lemon - 0.9/1L</t>
+  </si>
+  <si>
+    <t>Panoramic Photo; SS_Panoramic Photo</t>
+  </si>
+  <si>
+    <t>Dobry 0.2; SS_Dobry 0.2</t>
+  </si>
+  <si>
+    <t>Dobry 0.2_Zone; SS_Dobry 0.2_Zone</t>
+  </si>
+  <si>
+    <t>Entry_Pack; SS_Dobry 0.2_Zone</t>
+  </si>
+  <si>
+    <t>Entry_PacK_ Zone; SS_Dobry 0.2_Zone</t>
+  </si>
+  <si>
+    <t>Panoramic photo of Cooler; SS_Panoramic photo of Cooler - Traditional Trade</t>
+  </si>
+  <si>
+    <t>SSD 1 door; SSD 1.5 door; Mixed 1 door; Mixed  1.5 door; SS_SSD 1 door; SS_SSD 1.5 door; SS_Mixed 1 door; SS_Mixed  1.5 door</t>
+  </si>
+  <si>
+    <t>SSD 1 door; NCB 1 door; Mixed 1 door; SSD 1.5 door; NSB  1.5 door; Mixed  1.5 door; SSDFL 1 door; SSDFL 1.5 door; SS_SSD 1 door; SS_NCB 1 door; SS_Mixed 1 door; SS_SSD 1.5 door; SS_NSB  1.5 door; SS_Mixed  1.5 door; SS_SSDFL 1 door; SS_SSDFL 1.5 door</t>
+  </si>
+  <si>
+    <t>SSD 1 door; NSB 1 door; Mixed 1 door; FC 1 door; SSD 1.5 door; NSB  1.5 door; Mixed  1.5 door; FC door 1.5 door</t>
+  </si>
+  <si>
+    <t>Freezer BIG SSD; SSD Cooler-Side Rack Big; SSD Cooler-Side Rack Small; SSD Mini pallet; SSD Neck-hanging Rack; Freezer Small SSD; Other SSD Display BIG; Other SSD Display Small; Juice Cooler-Side Rack; Juice Freezer; Juice Mini Pallet; Other Juice Display BIG; Pulpy Cooler-Side Rack; Pulpy Other; Other Juice Display Small; Bonaqua Display; Fuzetea Display; Energy Display; Promo SSD; Promo Juice; Promo Water; Promo Energy; Promo Fuzetea</t>
   </si>
 </sst>
 </file>
@@ -1823,58 +1823,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AML103"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="I1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="T1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="P18" sqref="O18:P18"/>
+      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1:AA1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="3"/>
-    <col min="2" max="2" width="15.5703125" style="3"/>
-    <col min="3" max="3" width="25.7109375" style="3"/>
+    <col min="1" max="1" width="13.6640625" style="3"/>
+    <col min="2" max="2" width="15.5546875" style="3"/>
+    <col min="3" max="3" width="25.6640625" style="3"/>
     <col min="4" max="4" width="15" style="3"/>
-    <col min="5" max="5" width="20.85546875" style="3"/>
-    <col min="6" max="6" width="64.28515625" style="3"/>
-    <col min="7" max="7" width="91.7109375" style="3"/>
-    <col min="8" max="8" width="58.28515625" style="3"/>
+    <col min="5" max="5" width="20.88671875" style="3"/>
+    <col min="6" max="6" width="64.33203125" style="3"/>
+    <col min="7" max="7" width="91.6640625" style="3"/>
+    <col min="8" max="8" width="58.33203125" style="3"/>
     <col min="9" max="9" width="25" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" style="3"/>
-    <col min="12" max="12" width="12.42578125" style="3"/>
-    <col min="13" max="13" width="18.140625" style="3"/>
-    <col min="14" max="14" width="19.28515625" style="3"/>
-    <col min="15" max="15" width="31.140625" style="3"/>
-    <col min="16" max="16" width="97.28515625" style="3"/>
+    <col min="10" max="10" width="25.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" style="3"/>
+    <col min="12" max="12" width="12.44140625" style="3"/>
+    <col min="13" max="13" width="18.109375" style="3"/>
+    <col min="14" max="14" width="19.33203125" style="3"/>
+    <col min="15" max="15" width="31.109375" style="3"/>
+    <col min="16" max="16" width="97.33203125" style="3"/>
     <col min="17" max="17" width="27" style="3"/>
-    <col min="18" max="18" width="13.28515625" style="3"/>
+    <col min="18" max="18" width="13.33203125" style="3"/>
     <col min="19" max="19" width="26" style="3"/>
-    <col min="20" max="20" width="18.5703125" style="3"/>
-    <col min="21" max="21" width="10.7109375" style="3"/>
-    <col min="22" max="22" width="19.7109375" style="3"/>
-    <col min="23" max="23" width="24.140625" style="3"/>
-    <col min="24" max="24" width="30.85546875" style="3"/>
-    <col min="25" max="25" width="29.85546875" style="3"/>
-    <col min="26" max="26" width="65.28515625" style="3"/>
-    <col min="27" max="27" width="32.28515625" style="3"/>
-    <col min="28" max="28" width="34.7109375" style="3"/>
+    <col min="20" max="20" width="18.5546875" style="3"/>
+    <col min="21" max="21" width="10.6640625" style="3"/>
+    <col min="22" max="22" width="19.6640625" style="3"/>
+    <col min="23" max="23" width="24.109375" style="3"/>
+    <col min="24" max="24" width="30.88671875" style="3"/>
+    <col min="25" max="25" width="29.88671875" style="3"/>
+    <col min="26" max="26" width="65.33203125" style="3"/>
+    <col min="27" max="27" width="32.33203125" style="3"/>
+    <col min="28" max="28" width="34.6640625" style="3"/>
     <col min="29" max="29" width="36" style="3"/>
-    <col min="30" max="31" width="21.5703125" style="3"/>
-    <col min="32" max="32" width="18.140625" style="3"/>
-    <col min="33" max="33" width="17.28515625" style="3"/>
-    <col min="34" max="34" width="17.7109375" style="3"/>
-    <col min="35" max="35" width="33.28515625" style="3"/>
-    <col min="36" max="36" width="114.28515625" style="3"/>
-    <col min="37" max="37" width="10.28515625" style="3"/>
+    <col min="30" max="31" width="21.5546875" style="3"/>
+    <col min="32" max="32" width="18.109375" style="3"/>
+    <col min="33" max="33" width="17.33203125" style="3"/>
+    <col min="34" max="34" width="17.6640625" style="3"/>
+    <col min="35" max="35" width="33.33203125" style="3"/>
+    <col min="36" max="36" width="114.33203125" style="3"/>
+    <col min="37" max="37" width="10.33203125" style="3"/>
     <col min="38" max="38" width="12" style="3"/>
-    <col min="39" max="39" width="14.7109375" style="3"/>
-    <col min="40" max="40" width="13.140625" style="3"/>
+    <col min="39" max="39" width="14.6640625" style="3"/>
+    <col min="40" max="40" width="13.109375" style="3"/>
     <col min="41" max="1026" width="12" style="3"/>
-    <col min="1027" max="16384" width="8.85546875" style="4"/>
+    <col min="1027" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1025" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1900,10 +1900,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1996,7 +1996,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3045,7 +3045,7 @@
       <c r="AMJ2" s="4"/>
       <c r="AMK2" s="4"/>
     </row>
-    <row r="3" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3173,7 +3173,7 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
       <c r="AA4" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB4" s="4"/>
       <c r="AC4" s="4"/>
@@ -3199,7 +3199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3254,7 +3254,7 @@
       <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
       <c r="AA5" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
@@ -3280,7 +3280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3335,7 +3335,7 @@
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
       <c r="AA6" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB6" s="4"/>
       <c r="AC6" s="4"/>
@@ -3361,7 +3361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3416,7 +3416,7 @@
       <c r="Y7" s="4"/>
       <c r="Z7" s="4"/>
       <c r="AA7" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB7" s="4"/>
       <c r="AC7" s="4"/>
@@ -3442,7 +3442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3497,7 +3497,7 @@
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
       <c r="AA8" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
@@ -3523,7 +3523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3578,7 +3578,7 @@
       <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
       <c r="AA9" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB9" s="4"/>
       <c r="AC9" s="4"/>
@@ -3604,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3659,7 +3659,7 @@
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
       <c r="AA10" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
@@ -3685,7 +3685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3740,7 +3740,7 @@
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
       <c r="AA11" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
@@ -3766,7 +3766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -3821,7 +3821,7 @@
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
       <c r="AA12" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
@@ -3847,7 +3847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3902,7 +3902,7 @@
       <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
       <c r="AA13" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB13" s="4"/>
       <c r="AC13" s="4"/>
@@ -3928,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3983,7 +3983,7 @@
       <c r="Y14" s="4"/>
       <c r="Z14" s="4"/>
       <c r="AA14" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
@@ -4009,7 +4009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -4064,7 +4064,7 @@
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
       <c r="AA15" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
@@ -4090,7 +4090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1025" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -4145,7 +4145,7 @@
       <c r="Y16" s="4"/>
       <c r="Z16" s="4"/>
       <c r="AA16" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
@@ -4171,7 +4171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -4226,7 +4226,7 @@
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
       <c r="AA17" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
@@ -4252,7 +4252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -4285,10 +4285,10 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="9" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="P18" s="9" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
@@ -4307,7 +4307,7 @@
       <c r="Y18" s="4"/>
       <c r="Z18" s="4"/>
       <c r="AA18" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB18" s="4"/>
       <c r="AC18" s="4"/>
@@ -4333,7 +4333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4388,7 +4388,7 @@
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
       <c r="AA19" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
@@ -4414,7 +4414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -4469,7 +4469,7 @@
       <c r="Y20" s="4"/>
       <c r="Z20" s="4"/>
       <c r="AA20" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
@@ -4495,7 +4495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -4550,7 +4550,7 @@
       <c r="Y21" s="4"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
@@ -4576,7 +4576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -4631,7 +4631,7 @@
       <c r="Y22" s="4"/>
       <c r="Z22" s="4"/>
       <c r="AA22" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
@@ -4657,7 +4657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>28</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>29</v>
       </c>
@@ -4785,7 +4785,7 @@
       <c r="Y24" s="4"/>
       <c r="Z24" s="4"/>
       <c r="AA24" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
@@ -4811,7 +4811,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>30</v>
       </c>
@@ -4866,7 +4866,7 @@
       <c r="Y25" s="4"/>
       <c r="Z25" s="4"/>
       <c r="AA25" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
@@ -4892,7 +4892,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>31</v>
       </c>
@@ -4947,7 +4947,7 @@
       <c r="Y26" s="4"/>
       <c r="Z26" s="4"/>
       <c r="AA26" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
@@ -4973,7 +4973,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>32</v>
       </c>
@@ -5028,7 +5028,7 @@
       <c r="Y27" s="4"/>
       <c r="Z27" s="4"/>
       <c r="AA27" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
@@ -5054,7 +5054,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>35</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>36</v>
       </c>
@@ -5182,7 +5182,7 @@
       <c r="Y29" s="4"/>
       <c r="Z29" s="4"/>
       <c r="AA29" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB29" s="4"/>
       <c r="AC29" s="4"/>
@@ -5208,7 +5208,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>37</v>
       </c>
@@ -5263,7 +5263,7 @@
       <c r="Y30" s="4"/>
       <c r="Z30" s="4"/>
       <c r="AA30" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB30" s="4"/>
       <c r="AC30" s="4"/>
@@ -5289,7 +5289,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>38</v>
       </c>
@@ -5344,7 +5344,7 @@
       <c r="Y31" s="4"/>
       <c r="Z31" s="4"/>
       <c r="AA31" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB31" s="4"/>
       <c r="AC31" s="4"/>
@@ -5370,7 +5370,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>39</v>
       </c>
@@ -5425,7 +5425,7 @@
       <c r="Y32" s="4"/>
       <c r="Z32" s="4"/>
       <c r="AA32" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB32" s="4"/>
       <c r="AC32" s="4"/>
@@ -5451,7 +5451,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>40</v>
       </c>
@@ -5506,7 +5506,7 @@
       <c r="Y33" s="4"/>
       <c r="Z33" s="4"/>
       <c r="AA33" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB33" s="4"/>
       <c r="AC33" s="4"/>
@@ -5532,7 +5532,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>42</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="35" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>43</v>
       </c>
@@ -5660,7 +5660,7 @@
       <c r="Y35" s="4"/>
       <c r="Z35" s="4"/>
       <c r="AA35" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB35" s="4"/>
       <c r="AC35" s="4"/>
@@ -5686,7 +5686,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>44</v>
       </c>
@@ -5741,7 +5741,7 @@
       <c r="Y36" s="4"/>
       <c r="Z36" s="4"/>
       <c r="AA36" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB36" s="4"/>
       <c r="AC36" s="4"/>
@@ -5767,7 +5767,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>45</v>
       </c>
@@ -5822,7 +5822,7 @@
       <c r="Y37" s="4"/>
       <c r="Z37" s="4"/>
       <c r="AA37" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB37" s="4"/>
       <c r="AC37" s="4"/>
@@ -5848,7 +5848,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>46</v>
       </c>
@@ -5903,7 +5903,7 @@
       <c r="Y38" s="4"/>
       <c r="Z38" s="4"/>
       <c r="AA38" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB38" s="4"/>
       <c r="AC38" s="4"/>
@@ -5929,7 +5929,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>49</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="40" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>50</v>
       </c>
@@ -6056,7 +6056,7 @@
       <c r="Y40" s="4"/>
       <c r="Z40" s="4"/>
       <c r="AA40" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB40" s="4"/>
       <c r="AC40" s="4"/>
@@ -6082,7 +6082,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>51</v>
       </c>
@@ -6136,7 +6136,7 @@
       <c r="Y41" s="4"/>
       <c r="Z41" s="4"/>
       <c r="AA41" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB41" s="4"/>
       <c r="AC41" s="4"/>
@@ -6162,7 +6162,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>52</v>
       </c>
@@ -6216,7 +6216,7 @@
       <c r="Y42" s="4"/>
       <c r="Z42" s="4"/>
       <c r="AA42" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB42" s="4"/>
       <c r="AC42" s="4"/>
@@ -6242,7 +6242,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>53</v>
       </c>
@@ -6296,7 +6296,7 @@
       <c r="Y43" s="4"/>
       <c r="Z43" s="4"/>
       <c r="AA43" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB43" s="4"/>
       <c r="AC43" s="4"/>
@@ -6322,7 +6322,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>54</v>
       </c>
@@ -6376,7 +6376,7 @@
       <c r="Y44" s="4"/>
       <c r="Z44" s="4"/>
       <c r="AA44" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB44" s="4"/>
       <c r="AC44" s="4"/>
@@ -6402,7 +6402,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>55</v>
       </c>
@@ -6456,7 +6456,7 @@
       <c r="Y45" s="4"/>
       <c r="Z45" s="4"/>
       <c r="AA45" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB45" s="4"/>
       <c r="AC45" s="4"/>
@@ -6482,7 +6482,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>56</v>
       </c>
@@ -6536,7 +6536,7 @@
       <c r="Y46" s="4"/>
       <c r="Z46" s="4"/>
       <c r="AA46" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB46" s="4"/>
       <c r="AC46" s="4"/>
@@ -6562,7 +6562,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>57</v>
       </c>
@@ -6616,7 +6616,7 @@
       <c r="Y47" s="4"/>
       <c r="Z47" s="4"/>
       <c r="AA47" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB47" s="4"/>
       <c r="AC47" s="4"/>
@@ -6642,7 +6642,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>58</v>
       </c>
@@ -6696,7 +6696,7 @@
       <c r="Y48" s="4"/>
       <c r="Z48" s="4"/>
       <c r="AA48" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB48" s="4"/>
       <c r="AC48" s="4"/>
@@ -6722,7 +6722,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>59</v>
       </c>
@@ -6776,7 +6776,7 @@
       <c r="Y49" s="4"/>
       <c r="Z49" s="4"/>
       <c r="AA49" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AB49" s="4"/>
       <c r="AC49" s="4"/>
@@ -6802,7 +6802,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>62</v>
       </c>
@@ -6861,7 +6861,7 @@
       </c>
       <c r="AN50" s="4"/>
     </row>
-    <row r="51" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>63</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="52" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>64</v>
       </c>
@@ -6988,7 +6988,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="53" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>65</v>
       </c>
@@ -7042,7 +7042,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="54" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>66</v>
       </c>
@@ -7108,7 +7108,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="55" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>67</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="56" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>68</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="57" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>69</v>
       </c>
@@ -7282,7 +7282,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="58" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>70</v>
       </c>
@@ -7348,7 +7348,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="59" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>71</v>
       </c>
@@ -7402,7 +7402,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="60" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>72</v>
       </c>
@@ -7468,7 +7468,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="61" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>73</v>
       </c>
@@ -7520,7 +7520,7 @@
       </c>
       <c r="AN61" s="4"/>
     </row>
-    <row r="62" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>74</v>
       </c>
@@ -7574,7 +7574,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="63" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>75</v>
       </c>
@@ -7641,7 +7641,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="64" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>76</v>
       </c>
@@ -7709,7 +7709,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>77</v>
       </c>
@@ -7773,7 +7773,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>78</v>
       </c>
@@ -7841,7 +7841,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>80</v>
       </c>
@@ -7895,7 +7895,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="68" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>81</v>
       </c>
@@ -7962,7 +7962,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="69" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>82</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>83</v>
       </c>
@@ -8094,7 +8094,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>84</v>
       </c>
@@ -8162,7 +8162,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>85</v>
       </c>
@@ -8230,7 +8230,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>86</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="74" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>87</v>
       </c>
@@ -8340,7 +8340,7 @@
       </c>
       <c r="Y74" s="4"/>
       <c r="Z74" s="3" t="s">
-        <v>273</v>
+        <v>394</v>
       </c>
       <c r="AA74" s="4"/>
       <c r="AD74" s="4"/>
@@ -8361,7 +8361,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>88</v>
       </c>
@@ -8374,13 +8374,13 @@
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
       <c r="F75" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="G75" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="G75" s="3" t="s">
+      <c r="H75" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="H75" s="3" t="s">
-        <v>276</v>
       </c>
       <c r="K75" s="4"/>
       <c r="L75" s="3">
@@ -8393,11 +8393,11 @@
       <c r="R75" s="4"/>
       <c r="S75" s="4"/>
       <c r="T75" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Y75" s="4"/>
       <c r="Z75" s="3" t="s">
-        <v>278</v>
+        <v>395</v>
       </c>
       <c r="AA75" s="4"/>
       <c r="AD75" s="4"/>
@@ -8409,7 +8409,7 @@
         <v>268</v>
       </c>
       <c r="AJ75" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AK75" s="3">
         <v>3</v>
@@ -8422,7 +8422,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>89</v>
       </c>
@@ -8435,10 +8435,10 @@
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
       <c r="F76" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>51</v>
@@ -8450,10 +8450,10 @@
       <c r="M76" s="4"/>
       <c r="N76" s="4"/>
       <c r="O76" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="P76" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="R76" s="4"/>
       <c r="S76" s="3" t="s">
@@ -8464,7 +8464,7 @@
       </c>
       <c r="Y76" s="4"/>
       <c r="Z76" s="3" t="s">
-        <v>284</v>
+        <v>396</v>
       </c>
       <c r="AA76" s="4"/>
       <c r="AD76" s="4"/>
@@ -8485,7 +8485,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>90</v>
       </c>
@@ -8498,13 +8498,13 @@
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
       <c r="F77" s="3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K77" s="4"/>
       <c r="L77" s="3">
@@ -8517,11 +8517,11 @@
       <c r="R77" s="4"/>
       <c r="S77" s="4"/>
       <c r="T77" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Y77" s="4"/>
       <c r="Z77" s="3" t="s">
-        <v>287</v>
+        <v>397</v>
       </c>
       <c r="AA77" s="4"/>
       <c r="AD77" s="4"/>
@@ -8530,10 +8530,10 @@
       </c>
       <c r="AF77" s="4"/>
       <c r="AI77" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="AJ77" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="AK77" s="3">
         <v>3</v>
@@ -8546,7 +8546,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>91</v>
       </c>
@@ -8561,10 +8561,10 @@
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>40</v>
@@ -8593,11 +8593,11 @@
         <v>310</v>
       </c>
       <c r="AM78" s="6" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="AN78" s="4"/>
     </row>
-    <row r="79" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>92</v>
       </c>
@@ -8612,10 +8612,10 @@
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>40</v>
@@ -8650,7 +8650,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="80" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>93</v>
       </c>
@@ -8664,16 +8664,16 @@
         <v>40</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="K80" s="4"/>
       <c r="L80" s="4"/>
@@ -8683,7 +8683,7 @@
       <c r="P80" s="4"/>
       <c r="R80" s="4"/>
       <c r="S80" s="3" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="T80" s="4"/>
       <c r="Y80" s="4"/>
@@ -8698,7 +8698,7 @@
       </c>
       <c r="AI80" s="4"/>
       <c r="AJ80" s="3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="AK80" s="3">
         <v>2</v>
@@ -8707,13 +8707,13 @@
         <v>79</v>
       </c>
       <c r="AM80" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="AN80" s="3">
         <v>311</v>
       </c>
     </row>
-    <row r="81" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>94</v>
       </c>
@@ -8727,16 +8727,16 @@
         <v>40</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="K81" s="4"/>
       <c r="L81" s="3">
@@ -8747,18 +8747,18 @@
       </c>
       <c r="N81" s="4"/>
       <c r="O81" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="P81" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="R81" s="4"/>
       <c r="S81" s="4"/>
       <c r="T81" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="Y81" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Z81" s="4"/>
       <c r="AA81" s="4"/>
@@ -8768,10 +8768,10 @@
       </c>
       <c r="AF81" s="4"/>
       <c r="AI81" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="AJ81" s="3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="AK81" s="3">
         <v>3</v>
@@ -8784,7 +8784,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>96</v>
       </c>
@@ -8798,16 +8798,16 @@
         <v>40</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="K82" s="4"/>
       <c r="L82" s="3">
@@ -8819,15 +8819,15 @@
         <v>201</v>
       </c>
       <c r="P82" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="R82" s="4"/>
       <c r="S82" s="4"/>
       <c r="T82" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="Y82" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="Z82" s="4"/>
       <c r="AA82" s="4"/>
@@ -8849,7 +8849,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>97</v>
       </c>
@@ -8864,10 +8864,10 @@
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="H83" s="3" t="s">
         <v>40</v>
@@ -8896,13 +8896,13 @@
         <v>312</v>
       </c>
       <c r="AM83" s="6" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="AN83" s="3">
         <v>310</v>
       </c>
     </row>
-    <row r="84" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>98</v>
       </c>
@@ -8919,13 +8919,13 @@
         <v>263</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K84" s="4"/>
       <c r="L84" s="3">
@@ -8935,15 +8935,15 @@
       <c r="N84" s="4"/>
       <c r="O84" s="4"/>
       <c r="P84" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="R84" s="4"/>
       <c r="S84" s="4"/>
       <c r="T84" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Y84" s="3" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="Z84" s="3" t="s">
         <v>398</v>
@@ -8957,10 +8957,10 @@
         <v>0.03</v>
       </c>
       <c r="AI84" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="AJ84" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="AK84" s="3">
         <v>2</v>
@@ -8973,7 +8973,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="85" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>99</v>
       </c>
@@ -8990,13 +8990,13 @@
         <v>263</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="K85" s="4"/>
       <c r="L85" s="4"/>
@@ -9007,18 +9007,18 @@
         <v>15</v>
       </c>
       <c r="O85" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="P85" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="R85" s="4"/>
       <c r="S85" s="4"/>
       <c r="T85" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="Y85" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Z85" s="4"/>
       <c r="AD85" s="4"/>
@@ -9029,10 +9029,10 @@
         <v>0.03</v>
       </c>
       <c r="AI85" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="AJ85" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="AK85" s="3">
         <v>2</v>
@@ -9045,7 +9045,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="86" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>100</v>
       </c>
@@ -9062,10 +9062,10 @@
         <v>263</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>47</v>
@@ -9080,7 +9080,7 @@
       </c>
       <c r="T86" s="4"/>
       <c r="Y86" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Z86" s="4"/>
       <c r="AD86" s="4"/>
@@ -9091,10 +9091,10 @@
         <v>0.03</v>
       </c>
       <c r="AI86" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="AJ86" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="AK86" s="3">
         <v>2</v>
@@ -9103,13 +9103,13 @@
         <v>85</v>
       </c>
       <c r="AM86" s="6" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="AN86" s="3">
         <v>312</v>
       </c>
     </row>
-    <row r="87" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>101</v>
       </c>
@@ -9124,26 +9124,26 @@
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="K87" s="4"/>
       <c r="L87" s="3">
         <v>0.4</v>
       </c>
       <c r="O87" s="3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="P87" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="R87" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="S87" s="3" t="s">
         <v>54</v>
@@ -9152,10 +9152,10 @@
         <v>271</v>
       </c>
       <c r="Y87" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Z87" s="3" t="s">
-        <v>333</v>
+        <v>399</v>
       </c>
       <c r="AD87" s="4"/>
       <c r="AE87" s="3" t="s">
@@ -9163,10 +9163,10 @@
       </c>
       <c r="AF87" s="4"/>
       <c r="AI87" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="AJ87" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="AK87" s="3">
         <v>3</v>
@@ -9179,7 +9179,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>102</v>
       </c>
@@ -9194,10 +9194,10 @@
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="3" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>240</v>
@@ -9214,7 +9214,7 @@
       </c>
       <c r="T88" s="4"/>
       <c r="Y88" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Z88" s="4"/>
       <c r="AD88" s="4"/>
@@ -9223,10 +9223,10 @@
       </c>
       <c r="AF88" s="4"/>
       <c r="AI88" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="AJ88" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="AK88" s="3">
         <v>3</v>
@@ -9235,13 +9235,13 @@
         <v>88</v>
       </c>
       <c r="AM88" s="6" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="AN88" s="3">
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>103</v>
       </c>
@@ -9256,10 +9256,10 @@
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="3" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>51</v>
@@ -9269,13 +9269,13 @@
         <v>4</v>
       </c>
       <c r="O89" s="3" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="P89" s="3" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="R89" s="3" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="S89" s="3" t="s">
         <v>54</v>
@@ -9284,23 +9284,23 @@
         <v>271</v>
       </c>
       <c r="Y89" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Z89" s="6" t="s">
-        <v>341</v>
+        <v>400</v>
       </c>
       <c r="AD89" s="3" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="AE89" s="3" t="s">
         <v>57</v>
       </c>
       <c r="AF89" s="4"/>
       <c r="AI89" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="AJ89" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="AK89" s="3">
         <v>4</v>
@@ -9313,7 +9313,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>104</v>
       </c>
@@ -9328,10 +9328,10 @@
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="3" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>51</v>
@@ -9341,13 +9341,13 @@
         <v>4</v>
       </c>
       <c r="O90" s="3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="P90" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="R90" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="S90" s="3" t="s">
         <v>54</v>
@@ -9356,23 +9356,23 @@
         <v>271</v>
       </c>
       <c r="Y90" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Z90" s="6" t="s">
-        <v>341</v>
+        <v>400</v>
       </c>
       <c r="AD90" s="3" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="AE90" s="3" t="s">
         <v>57</v>
       </c>
       <c r="AF90" s="4"/>
       <c r="AI90" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="AJ90" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="AK90" s="3">
         <v>4</v>
@@ -9385,7 +9385,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>105</v>
       </c>
@@ -9400,13 +9400,13 @@
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="3" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="K91" s="4"/>
       <c r="L91" s="3">
@@ -9416,29 +9416,29 @@
         <v>201</v>
       </c>
       <c r="P91" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="S91" s="3" t="s">
         <v>54</v>
       </c>
       <c r="T91" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="Y91" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Z91" s="6" t="s">
-        <v>341</v>
+        <v>400</v>
       </c>
       <c r="AE91" s="3" t="s">
         <v>57</v>
       </c>
       <c r="AF91" s="4"/>
       <c r="AI91" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="AJ91" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="AK91" s="3">
         <v>3</v>
@@ -9451,7 +9451,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>106</v>
       </c>
@@ -9468,24 +9468,24 @@
         <v>263</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="K92" s="4"/>
       <c r="O92" s="4"/>
       <c r="P92" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="T92" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="Y92" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Z92" s="4"/>
       <c r="AE92" s="3" t="s">
@@ -9495,10 +9495,10 @@
         <v>0.03</v>
       </c>
       <c r="AI92" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="AJ92" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="AK92" s="3">
         <v>2</v>
@@ -9511,7 +9511,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="93" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>107</v>
       </c>
@@ -9522,27 +9522,27 @@
         <v>39</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="K93" s="3" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="O93" s="4"/>
       <c r="P93" s="4"/>
       <c r="T93" s="3" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="Y93" s="4"/>
       <c r="Z93" s="4"/>
@@ -9550,10 +9550,10 @@
         <v>93</v>
       </c>
       <c r="AM93" s="6" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="94" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="94" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>108</v>
       </c>
@@ -9564,31 +9564,31 @@
         <v>39</v>
       </c>
       <c r="D94" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="K94" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="O94" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="P94" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="T94" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="G94" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="H94" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="K94" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="O94" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="P94" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="T94" s="3" t="s">
-        <v>357</v>
       </c>
       <c r="Y94" s="4"/>
       <c r="Z94" s="4"/>
@@ -9599,7 +9599,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>109</v>
       </c>
@@ -9610,31 +9610,31 @@
         <v>39</v>
       </c>
       <c r="D95" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="K95" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="O95" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="P95" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="T95" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="H95" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="K95" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="O95" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="P95" s="6" t="s">
-        <v>366</v>
-      </c>
-      <c r="T95" s="3" t="s">
-        <v>357</v>
       </c>
       <c r="Y95" s="4"/>
       <c r="Z95" s="4"/>
@@ -9645,7 +9645,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:40" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>110</v>
       </c>
@@ -9656,31 +9656,31 @@
         <v>39</v>
       </c>
       <c r="D96" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="K96" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="O96" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="P96" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="T96" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="K96" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="O96" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="P96" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="T96" s="3" t="s">
-        <v>357</v>
       </c>
       <c r="Y96" s="4"/>
       <c r="Z96" s="4"/>
@@ -9691,7 +9691,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="97" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>111</v>
       </c>
@@ -9702,31 +9702,31 @@
         <v>39</v>
       </c>
       <c r="D97" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="K97" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="O97" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="P97" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="T97" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="G97" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="H97" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="K97" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="O97" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="P97" s="6" t="s">
-        <v>368</v>
-      </c>
-      <c r="T97" s="3" t="s">
-        <v>357</v>
       </c>
       <c r="Y97" s="4"/>
       <c r="Z97" s="4"/>
@@ -9737,7 +9737,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="98" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>112</v>
       </c>
@@ -9748,42 +9748,42 @@
         <v>39</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="K98" s="3" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="O98" s="4"/>
       <c r="P98" s="3" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="T98" s="3" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="Y98" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Z98" s="6" t="s">
-        <v>375</v>
+        <v>401</v>
       </c>
       <c r="AL98" s="3">
         <v>98</v>
       </c>
       <c r="AM98" s="4"/>
     </row>
-    <row r="99" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>113</v>
       </c>
@@ -9794,39 +9794,39 @@
         <v>39</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="K99" s="3" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="O99" s="4"/>
       <c r="P99" s="3" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="T99" s="3" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="Z99" s="6" t="s">
-        <v>381</v>
+        <v>402</v>
       </c>
       <c r="AL99" s="3">
         <v>99</v>
       </c>
       <c r="AM99" s="4"/>
     </row>
-    <row r="100" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>114</v>
       </c>
@@ -9837,39 +9837,39 @@
         <v>39</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="K100" s="3" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="O100" s="4"/>
       <c r="P100" s="3" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="T100" s="3" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="Z100" s="6" t="s">
-        <v>381</v>
+        <v>402</v>
       </c>
       <c r="AL100" s="3">
         <v>101</v>
       </c>
       <c r="AM100" s="4"/>
     </row>
-    <row r="101" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>115</v>
       </c>
@@ -9880,40 +9880,40 @@
         <v>39</v>
       </c>
       <c r="D101" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="K101" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="O101" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="P101" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="T101" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="G101" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="H101" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="K101" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="O101" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="P101" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="T101" s="3" t="s">
-        <v>357</v>
       </c>
       <c r="AL101" s="3">
         <v>102</v>
       </c>
       <c r="AM101" s="6" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="102" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="102" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>116</v>
       </c>
@@ -9924,40 +9924,40 @@
         <v>39</v>
       </c>
       <c r="D102" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="K102" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="O102" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="P102" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="T102" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="G102" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="H102" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="K102" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="O102" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="P102" s="6" t="s">
-        <v>392</v>
-      </c>
-      <c r="T102" s="3" t="s">
-        <v>357</v>
       </c>
       <c r="AL102" s="3">
         <v>104</v>
       </c>
       <c r="AM102" s="6" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="103" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="103" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>117</v>
       </c>
@@ -9968,22 +9968,22 @@
         <v>39</v>
       </c>
       <c r="D103" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="H103" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="K103" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="T103" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="H103" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="K103" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="T103" s="3" t="s">
-        <v>357</v>
       </c>
       <c r="AL103" s="3">
         <v>521</v>

</xml_diff>